<commit_message>
Geracao do codigo binario
</commit_message>
<xml_diff>
--- a/conjunto de instrucoes.xlsx
+++ b/conjunto de instrucoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instruções" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
   <si>
     <t xml:space="preserve">INSTRUÇÃO</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t xml:space="preserve">ACESSO A MEMÓRIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOADR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS é um end de memória</t>
   </si>
   <si>
     <t xml:space="preserve">LOADI [RD, IM22]</t>
@@ -598,17 +610,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.8866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -919,13 +931,25 @@
       <c r="D22" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>24</v>
@@ -936,10 +960,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>25</v>
@@ -950,10 +974,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>26</v>
@@ -964,10 +988,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>27</v>
@@ -978,10 +1002,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>28</v>
@@ -992,10 +1016,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C28" s="5" t="n">
         <v>29</v>
@@ -1006,10 +1030,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>30</v>
@@ -1020,10 +1044,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>31</v>
@@ -1034,10 +1058,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>32</v>
@@ -1048,10 +1072,10 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>33</v>
@@ -1090,10 +1114,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="25.7246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="9" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
@@ -1106,7 +1130,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -1116,27 +1140,31 @@
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
       <c r="C2" s="8" t="s">
-        <v>75</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
       <c r="C3" s="8" t="s">
-        <v>76</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0"/>
       <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
@@ -1146,15 +1174,24 @@
         <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>78</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="D7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="D8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1175,108 +1212,125 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="24.502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="1.95546558704453"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="25.4817813765182"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="43.2388663967611"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="1.92712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="43.5991902834008"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
       <c r="D2" s="15" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
       <c r="D6" s="15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
       <c r="D7" s="15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="B8" s="0"/>
+      <c r="D8" s="0"/>
       <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="15" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>